<commit_message>
fixed mistakes that introduced nans in the rdf
</commit_message>
<xml_diff>
--- a/tests/catalog_ai.xlsx
+++ b/tests/catalog_ai.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="121">
   <si>
     <t xml:space="preserve">dcterms:title</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">DTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">cc-by 4.0</t>
@@ -655,7 +658,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="E3 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -723,7 +726,7 @@
   <dimension ref="A1:P1010"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,766 +810,771 @@
       <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F2" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F3" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="3"/>
       <c r="L3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O3" s="7"/>
       <c r="P3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="3"/>
       <c r="L4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="3"/>
       <c r="L5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O5" s="8"/>
       <c r="P5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="3"/>
       <c r="L6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J7" s="3"/>
       <c r="L7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="3"/>
       <c r="L8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J9" s="3"/>
       <c r="L9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J10" s="3"/>
       <c r="L10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J11" s="3"/>
       <c r="L11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J12" s="3"/>
       <c r="L12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J13" s="3"/>
       <c r="L13" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J14" s="3"/>
       <c r="L14" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J15" s="3"/>
       <c r="L15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J16" s="3"/>
       <c r="L16" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="3"/>
       <c r="L17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J18" s="3"/>
       <c r="L18" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J19" s="3"/>
       <c r="L19" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J20" s="3"/>
       <c r="L20" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J21" s="3"/>
       <c r="L21" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J22" s="3"/>
       <c r="L22" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J23" s="3"/>
       <c r="L23" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J24" s="3"/>
       <c r="L24" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J25" s="3"/>
       <c r="L25" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J26" s="3"/>
       <c r="L26" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J27" s="3"/>
       <c r="L27" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="3"/>
       <c r="L28" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J29" s="3"/>
       <c r="L29" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4519,6 +4527,10 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="test@example.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="test@example.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4537,7 +4549,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="E3 H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4559,10 +4571,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>12</v>
@@ -4571,7 +4583,7 @@
         <v>19</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4609,7 +4621,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="1" sqref="E3 F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4621,48 +4633,48 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="0" t="s">
-        <v>101</v>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>104</v>
+      <c r="D3" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4687,7 +4699,7 @@
   <dimension ref="A1:E1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E3 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4703,16 +4715,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7740,7 +7752,7 @@
   <dimension ref="A1:E1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E3 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7756,16 +7768,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11805,7 +11817,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="E3 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11850,99 +11862,104 @@
     </row>
     <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F2" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="test@example.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>